<commit_message>
fix issues with update reporting
</commit_message>
<xml_diff>
--- a/shiny/demo_files/9 - Around the World in Eighty Days.xlsx
+++ b/shiny/demo_files/9 - Around the World in Eighty Days.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/carlosyanez/GitHub Projects/Trello_Dashboard/shiny/demo_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98EDA4EF-6F9F-B841-855A-926A8338AA4D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AE9D276-5CB6-9C45-9EEB-8FBA78B995EA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16040" activeTab="1" xr2:uid="{508D2F90-EA77-1648-9F60-F8C5F1C0AD05}"/>
+    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16040" xr2:uid="{508D2F90-EA77-1648-9F60-F8C5F1C0AD05}"/>
   </bookViews>
   <sheets>
     <sheet name="Project_Details" sheetId="1" r:id="rId1"/>
@@ -260,7 +260,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="168" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -397,7 +397,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -780,7 +780,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4C239EB-6B83-2348-BD16-80D2A8CFA94A}">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A2" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
@@ -855,7 +855,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E54E1E8-CF98-E444-82DF-4BB84BBBE4AF}">
   <dimension ref="A1:H23"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="A17" sqref="A17:XFD24"/>
     </sheetView>
   </sheetViews>
@@ -1015,11 +1015,11 @@
         <v>18</v>
       </c>
       <c r="F6" s="11">
-        <f t="shared" ref="F6:F12" si="0">G5</f>
+        <f t="shared" ref="F6:F11" si="0">G5</f>
         <v>43930</v>
       </c>
       <c r="G6" s="11">
-        <f t="shared" ref="G6:G12" si="1">H6+F6</f>
+        <f t="shared" ref="G6:G11" si="1">H6+F6</f>
         <v>43933</v>
       </c>
       <c r="H6" s="18">
@@ -1256,7 +1256,7 @@
   <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1332,7 +1332,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="11">
         <v>43966</v>
       </c>

</xml_diff>